<commit_message>
Modificación del LEF con creación inicial de personas por piso.
</commit_message>
<xml_diff>
--- a/LEF Simulación.xlsx
+++ b/LEF Simulación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisfemm\Documents\SimulacionAscensor-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisfemm\Documents\SimulacionAscensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
     <author>Luisfemm</author>
   </authors>
   <commentList>
-    <comment ref="R4" authorId="0" shapeId="0">
+    <comment ref="Y4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>LEF</t>
   </si>
@@ -125,23 +125,59 @@
     <t>En Movimiento</t>
   </si>
   <si>
-    <t>[{la, 146, 2}, {la, 246, 3}]</t>
-  </si>
-  <si>
-    <t>[{la,  0, 1}, {lp, 26, 3}]</t>
-  </si>
-  <si>
-    <t>[{lp, 26, 3}, {la, 146, 2}]</t>
-  </si>
-  <si>
     <t>[{la, 246, 3}, {lp, 277, 5}]</t>
+  </si>
+  <si>
+    <t>pisoOri</t>
+  </si>
+  <si>
+    <t>colaSubida4</t>
+  </si>
+  <si>
+    <t>colaSubida5</t>
+  </si>
+  <si>
+    <t>colaSubida6</t>
+  </si>
+  <si>
+    <t>colaBajada4</t>
+  </si>
+  <si>
+    <t>colaBajada5</t>
+  </si>
+  <si>
+    <t>colaBajada6</t>
+  </si>
+  <si>
+    <t>[{la,  0, 1}, {lp, 0, 3}]</t>
+  </si>
+  <si>
+    <t>[{lp,  0, 3}, {lp, 0, 6}]</t>
+  </si>
+  <si>
+    <t>[{lp, 0, 6}, {lp, 0, 1}]</t>
+  </si>
+  <si>
+    <t>[{lp, 0, 1}, {lp, 0, 5}]</t>
+  </si>
+  <si>
+    <t>[{lp, 0, 5}, {lp, 0, 1}]</t>
+  </si>
+  <si>
+    <t>[{lp,  0, 1}, {lp, 0, 4}]</t>
+  </si>
+  <si>
+    <t>[{lp, 0, 4}, {la, 121, 2}]</t>
+  </si>
+  <si>
+    <t>[{la, 121, 2}, {la, 245, 3}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +208,18 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Liberation Serif"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,12 +241,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,100 +541,129 @@
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+    <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="R3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="S3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="T3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="V3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="W3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="X3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="Y3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -613,34 +692,55 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>20</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <v>100</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
         <v>16</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="X4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" t="s">
+      <c r="Y4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -669,101 +769,143 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>20</v>
       </c>
-      <c r="L5">
+      <c r="R5">
         <v>100</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
         <v>16</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>23</v>
+      </c>
+      <c r="X5" t="s">
         <v>19</v>
       </c>
-      <c r="R5" t="s">
-        <v>26</v>
+      <c r="Y5" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
         <v>20</v>
       </c>
-      <c r="C6">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>20</v>
-      </c>
-      <c r="L6">
+      <c r="R6">
         <v>100</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" t="s">
         <v>19</v>
       </c>
-      <c r="R6" t="s">
-        <v>27</v>
+      <c r="Y6" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -781,103 +923,530 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
         <v>20</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <v>100</v>
       </c>
-      <c r="M7">
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
         <v>2</v>
       </c>
-      <c r="N7">
-        <v>3</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="U7" t="s">
+        <v>16</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" t="s">
         <v>19</v>
       </c>
-      <c r="R7" t="s">
-        <v>25</v>
+      <c r="Y7" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>20</v>
+      </c>
+      <c r="R8">
         <v>100</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8" t="s">
+        <v>16</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
+        <v>23</v>
+      </c>
+      <c r="X8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
         <v>20</v>
       </c>
-      <c r="L8">
+      <c r="R9">
         <v>100</v>
       </c>
-      <c r="M8">
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>20</v>
+      </c>
+      <c r="R10">
+        <v>100</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10" t="s">
+        <v>16</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <v>100</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>6</v>
+      </c>
+      <c r="U11">
         <v>3</v>
       </c>
-      <c r="N8">
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>120</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>20</v>
+      </c>
+      <c r="R12">
+        <v>100</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="U12">
         <v>3</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12" t="s">
+        <v>24</v>
+      </c>
+      <c r="X12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>246</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>20</v>
+      </c>
+      <c r="R13">
+        <v>100</v>
+      </c>
+      <c r="S13">
+        <v>3</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="X13" t="s">
         <v>19</v>
       </c>
-      <c r="R8" t="s">
-        <v>28</v>
+      <c r="Y13" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>277</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C14">
         <v>31</v>
       </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="10:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cambios Proyecto netbeans y lef
</commit_message>
<xml_diff>
--- a/LEF Simulación.xlsx
+++ b/LEF Simulación.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisfemm\Documents\SimulacionAscensor-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\GitHub\SimulacionAscensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="LEF Sergio" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>LEF</t>
   </si>
@@ -135,6 +136,108 @@
   </si>
   <si>
     <t>[{la, 246, 3}, {lp, 277, 5}]</t>
+  </si>
+  <si>
+    <t>evento actual</t>
+  </si>
+  <si>
+    <t>atendidos</t>
+  </si>
+  <si>
+    <t>colabajada2</t>
+  </si>
+  <si>
+    <t>colasubida1</t>
+  </si>
+  <si>
+    <t>colasubida2</t>
+  </si>
+  <si>
+    <t>colasubida3</t>
+  </si>
+  <si>
+    <t>colabajada3</t>
+  </si>
+  <si>
+    <t>colabajada4</t>
+  </si>
+  <si>
+    <t>coladestino1</t>
+  </si>
+  <si>
+    <t>coladestino2</t>
+  </si>
+  <si>
+    <t>coladestino3</t>
+  </si>
+  <si>
+    <t>coladestino4</t>
+  </si>
+  <si>
+    <t>Colas de espera para ingresar al ascensor</t>
+  </si>
+  <si>
+    <t>colas con las personas que se bajan en cada piso</t>
+  </si>
+  <si>
+    <t>llegada de persona</t>
+  </si>
+  <si>
+    <t>ramdom llegadas</t>
+  </si>
+  <si>
+    <t>tiempo de llegada</t>
+  </si>
+  <si>
+    <t>ramdom pisodest</t>
+  </si>
+  <si>
+    <t>piso destino</t>
+  </si>
+  <si>
+    <t>piso inicial</t>
+  </si>
+  <si>
+    <t>dirDest</t>
+  </si>
+  <si>
+    <t>llegada del ascensor</t>
+  </si>
+  <si>
+    <t>tiempo de espera</t>
+  </si>
+  <si>
+    <t>capacidadOcupada</t>
+  </si>
+  <si>
+    <t>cola acum suben</t>
+  </si>
+  <si>
+    <t>lambda1</t>
+  </si>
+  <si>
+    <t>lambda2</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>pisoDestino</t>
+  </si>
+  <si>
+    <t>t arranque</t>
+  </si>
+  <si>
+    <t>desp entre pisos</t>
+  </si>
+  <si>
+    <t>tiempo e/s</t>
   </si>
 </sst>
 </file>
@@ -181,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,16 +292,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,80 +666,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -883,4 +1042,414 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="5" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="4">
+        <f ca="1">RAND()</f>
+        <v>0.95920501926980661</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="4">
+        <f ca="1">ROUND(-(1/B1)*LOG($D$1, EXP(1)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="4">
+        <f ca="1">RANDBETWEEN(1,9)</f>
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="4">
+        <v>4</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="4">
+        <v>20</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="4">
+        <f ca="1">ROUND(-(1/B2)*LOG($D$1, EXP(1)),0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="Q4:V4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge de archivos de Excel
</commit_message>
<xml_diff>
--- a/LEF Simulación.xlsx
+++ b/LEF Simulación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\GitHub\SimulacionAscensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisfemm\Documents\SimulacionAscensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -340,15 +340,10 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -357,7 +352,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
@@ -666,26 +666,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1074,369 +1074,372 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="2">
         <v>0.04</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="2">
         <f ca="1">RAND()</f>
-        <v>0.95920501926980661</v>
-      </c>
-      <c r="E1" s="4" t="s">
+        <v>1.5557323631888886E-2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="2">
         <f ca="1">ROUND(-(1/B1)*LOG($D$1, EXP(1)),0)</f>
-        <v>1</v>
-      </c>
-      <c r="H1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="2">
         <f ca="1">RANDBETWEEN(1,9)</f>
         <v>3</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="2">
         <v>4</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="2">
         <v>20</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="4">
+      <c r="P1" s="2">
         <v>100</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="4">
+      <c r="R1" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>0.02</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f ca="1">ROUND(-(1/B2)*LOG($D$1, EXP(1)),0)</f>
-        <v>2</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3" t="s">
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3" t="s">
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="X5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Y5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="Z5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AA5" s="3"/>
+      <c r="AA5" s="8"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="Q4:V4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="AA4:AA5"/>
@@ -1445,9 +1448,6 @@
     <mergeCell ref="G4:L4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="Q4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificaciones al código, creación de las personas en la inicialización. Modificaciones del LEF en Excel.
</commit_message>
<xml_diff>
--- a/LEF Simulación.xlsx
+++ b/LEF Simulación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisfemm\Documents\SimulacionAscensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\GitHub\SimulacionAscensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
   <si>
     <t>LEF</t>
   </si>
@@ -238,6 +238,126 @@
   </si>
   <si>
     <t>tiempo e/s</t>
+  </si>
+  <si>
+    <t>arriba</t>
+  </si>
+  <si>
+    <t>estadoAsc</t>
+  </si>
+  <si>
+    <t>cola acum bajan</t>
+  </si>
+  <si>
+    <t>&lt;&lt;[{P, 0}]&gt;&gt;</t>
+  </si>
+  <si>
+    <t>[{P, 0}]</t>
+  </si>
+  <si>
+    <t>{P,0}</t>
+  </si>
+  <si>
+    <t>[{P,0}]</t>
+  </si>
+  <si>
+    <t>abajo</t>
+  </si>
+  <si>
+    <t>[{P,0}, {A,0}]</t>
+  </si>
+  <si>
+    <t>Comienza el while</t>
+  </si>
+  <si>
+    <t>{A,0}</t>
+  </si>
+  <si>
+    <t>parado</t>
+  </si>
+  <si>
+    <t>marcha</t>
+  </si>
+  <si>
+    <t>[{A,0}]</t>
+  </si>
+  <si>
+    <t>[{P,9}, {A,121}]</t>
+  </si>
+  <si>
+    <t>{P, 9}</t>
+  </si>
+  <si>
+    <t>{A,121}</t>
+  </si>
+  <si>
+    <t>[{A,121}]</t>
+  </si>
+  <si>
+    <t>[{P,145},{A,221}]</t>
+  </si>
+  <si>
+    <t>{P,145}</t>
+  </si>
+  <si>
+    <t>{A,221}</t>
+  </si>
+  <si>
+    <t>[{A,221}]</t>
+  </si>
+  <si>
+    <t>[{P,243}{A,321}]</t>
+  </si>
+  <si>
+    <t>{P,243}</t>
+  </si>
+  <si>
+    <t>[{A,321}]</t>
+  </si>
+  <si>
+    <t>{A,321}</t>
+  </si>
+  <si>
+    <t>ramdon destino</t>
+  </si>
+  <si>
+    <t>[{P,370},{A, 442}]</t>
+  </si>
+  <si>
+    <t>{P,370}</t>
+  </si>
+  <si>
+    <t>[{A, 442}]</t>
+  </si>
+  <si>
+    <t>{A, 442}</t>
+  </si>
+  <si>
+    <t>[{A, 564},{P,592}]</t>
+  </si>
+  <si>
+    <t>{A, 564}</t>
+  </si>
+  <si>
+    <t>[{P,592}, {P,681},{A, 686}]</t>
+  </si>
+  <si>
+    <t>{P,592}</t>
+  </si>
+  <si>
+    <t>[{P,681},{A, 686}]</t>
+  </si>
+  <si>
+    <t>{P,681}</t>
+  </si>
+  <si>
+    <t>[{A, 686}]</t>
+  </si>
+  <si>
+    <t>{A,686}</t>
+  </si>
+  <si>
+    <t>[{P,698},{A, 809}]</t>
   </si>
 </sst>
 </file>
@@ -284,7 +404,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -333,23 +453,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -358,6 +639,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +941,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,26 +966,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1046,34 +1346,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AB29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W17" sqref="W17"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.85546875" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" customWidth="1"/>
     <col min="20" max="20" width="17.140625" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" customWidth="1"/>
-    <col min="26" max="26" width="23.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" customWidth="1"/>
+    <col min="27" max="27" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -1085,21 +1393,21 @@
       </c>
       <c r="D1" s="2">
         <f ca="1">RAND()</f>
-        <v>4.5471792314375925E-2</v>
+        <v>0.50819805997890932</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F1" s="2">
         <f ca="1">ROUND(-(1/B1)*LOG($D$1, EXP(1)),0)</f>
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>59</v>
       </c>
       <c r="I1" s="2">
-        <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>8</v>
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>17</v>
@@ -1125,8 +1433,14 @@
       <c r="R1" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -1138,67 +1452,69 @@
       </c>
       <c r="F2" s="2">
         <f ca="1">ROUND(-(1/B2)*LOG($D$1, EXP(1)),0)</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6" t="s">
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="2" t="s">
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1213,10 +1529,10 @@
       <c r="K5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="8" t="s">
         <v>37</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -1225,10 +1541,10 @@
       <c r="O5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="10" t="s">
         <v>44</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1237,207 +1553,1505 @@
       <c r="S5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" s="3" t="s">
+      <c r="T5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="U5" t="s">
         <v>47</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="V5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="W5" s="12" t="s">
         <v>10</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="Y5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="AA5" s="21"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1</v>
+      </c>
+      <c r="T6" s="2">
+        <v>4</v>
+      </c>
+      <c r="U6" s="2">
+        <v>4</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W6" s="8"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>2</v>
+      </c>
+      <c r="T7" s="5">
+        <v>7</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W7" s="8"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>3</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2</v>
+      </c>
+      <c r="U8" s="2">
+        <v>2</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W8" s="8"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>4</v>
+      </c>
+      <c r="T9" s="2">
+        <v>6</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W9" s="8">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="9">
+        <v>1</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" s="8">
+        <v>1</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0</v>
+      </c>
+      <c r="K11" s="14">
+        <v>1</v>
+      </c>
+      <c r="L11" s="17">
+        <v>1</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0</v>
+      </c>
+      <c r="N11" s="14">
+        <v>0</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0</v>
+      </c>
+      <c r="P11" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>9</v>
+      </c>
+      <c r="R11" s="14">
+        <v>9</v>
+      </c>
+      <c r="S11" s="14">
+        <v>1</v>
+      </c>
+      <c r="T11" s="14">
+        <v>2</v>
+      </c>
+      <c r="U11" s="14">
+        <v>2</v>
+      </c>
+      <c r="V11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="W11" s="16">
+        <v>2</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="2">
+        <v>2</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>121</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>24</v>
+      </c>
+      <c r="R13" s="2">
+        <v>145</v>
+      </c>
+      <c r="S13" s="2">
+        <v>2</v>
+      </c>
+      <c r="T13" s="2">
+        <v>4</v>
+      </c>
+      <c r="U13" s="2">
+        <v>4</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W13" s="2">
+        <v>3</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>145</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W14" s="2">
+        <v>3</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>221</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>22</v>
+      </c>
+      <c r="R15" s="2">
+        <v>243</v>
+      </c>
+      <c r="S15" s="2">
+        <v>3</v>
+      </c>
+      <c r="T15" s="2">
+        <v>7</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W15" s="2">
+        <v>4</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>243</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W16" s="2">
+        <v>4</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>321</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>49</v>
+      </c>
+      <c r="R17" s="2">
+        <v>370</v>
+      </c>
+      <c r="S17" s="2">
+        <v>4</v>
+      </c>
+      <c r="T17" s="2">
+        <v>2</v>
+      </c>
+      <c r="U17" s="2">
+        <v>2</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W17" s="2">
+        <v>3</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>370</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2">
+        <v>3</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>442</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>2</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>150</v>
+      </c>
+      <c r="R19" s="2">
+        <v>592</v>
+      </c>
+      <c r="S19" s="2">
+        <v>3</v>
+      </c>
+      <c r="T19" s="2">
+        <v>5</v>
+      </c>
+      <c r="U19" s="2">
+        <v>1</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W19" s="2">
+        <v>2</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>564</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>2</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>117</v>
+      </c>
+      <c r="R20" s="2">
+        <v>681</v>
+      </c>
+      <c r="S20" s="2">
+        <v>2</v>
+      </c>
+      <c r="T20" s="2">
+        <v>4</v>
+      </c>
+      <c r="U20" s="2">
+        <v>4</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W20" s="2">
+        <v>1</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>592</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>2</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2">
+        <v>1</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>681</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <v>2</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2">
+        <v>1</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>686</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>12</v>
+      </c>
+      <c r="R23" s="2">
+        <v>698</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2">
+        <v>2</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AA4:AA5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="G4:L4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="W4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correccion al modelo, para que no genere llegadas cuando alguien no se sube al ascensor EN SU DIRECCION, porque obviamente no va a parar si no se suben en la direccion en que va
</commit_message>
<xml_diff>
--- a/LEF Simulación.xlsx
+++ b/LEF Simulación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\GitHub\SimulacionAscensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\SimulacionAscensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
   <si>
     <t>LEF</t>
   </si>
@@ -141,39 +141,6 @@
     <t>evento actual</t>
   </si>
   <si>
-    <t>atendidos</t>
-  </si>
-  <si>
-    <t>colabajada2</t>
-  </si>
-  <si>
-    <t>colasubida1</t>
-  </si>
-  <si>
-    <t>colasubida2</t>
-  </si>
-  <si>
-    <t>colasubida3</t>
-  </si>
-  <si>
-    <t>colabajada3</t>
-  </si>
-  <si>
-    <t>colabajada4</t>
-  </si>
-  <si>
-    <t>coladestino1</t>
-  </si>
-  <si>
-    <t>coladestino2</t>
-  </si>
-  <si>
-    <t>coladestino3</t>
-  </si>
-  <si>
-    <t>coladestino4</t>
-  </si>
-  <si>
     <t>Colas de espera para ingresar al ascensor</t>
   </si>
   <si>
@@ -183,15 +150,9 @@
     <t>llegada de persona</t>
   </si>
   <si>
-    <t>ramdom llegadas</t>
-  </si>
-  <si>
     <t>tiempo de llegada</t>
   </si>
   <si>
-    <t>ramdom pisodest</t>
-  </si>
-  <si>
     <t>piso destino</t>
   </si>
   <si>
@@ -204,21 +165,12 @@
     <t>llegada del ascensor</t>
   </si>
   <si>
-    <t>tiempo de espera</t>
-  </si>
-  <si>
     <t>capacidadOcupada</t>
   </si>
   <si>
     <t>cola acum suben</t>
   </si>
   <si>
-    <t>lambda1</t>
-  </si>
-  <si>
-    <t>lambda2</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -228,15 +180,9 @@
     <t>a2</t>
   </si>
   <si>
-    <t>pisoDestino</t>
-  </si>
-  <si>
     <t>t arranque</t>
   </si>
   <si>
-    <t>desp entre pisos</t>
-  </si>
-  <si>
     <t>tiempo e/s</t>
   </si>
   <si>
@@ -276,88 +222,85 @@
     <t>parado</t>
   </si>
   <si>
-    <t>marcha</t>
-  </si>
-  <si>
-    <t>[{A,0}]</t>
-  </si>
-  <si>
-    <t>[{P,9}, {A,121}]</t>
-  </si>
-  <si>
-    <t>{P, 9}</t>
-  </si>
-  <si>
     <t>{A,121}</t>
   </si>
   <si>
     <t>[{A,121}]</t>
   </si>
   <si>
-    <t>[{P,145},{A,221}]</t>
-  </si>
-  <si>
-    <t>{P,145}</t>
-  </si>
-  <si>
-    <t>{A,221}</t>
-  </si>
-  <si>
-    <t>[{A,221}]</t>
-  </si>
-  <si>
-    <t>[{P,243}{A,321}]</t>
-  </si>
-  <si>
-    <t>{P,243}</t>
-  </si>
-  <si>
-    <t>[{A,321}]</t>
-  </si>
-  <si>
-    <t>{A,321}</t>
-  </si>
-  <si>
-    <t>ramdon destino</t>
-  </si>
-  <si>
-    <t>[{P,370},{A, 442}]</t>
-  </si>
-  <si>
-    <t>{P,370}</t>
-  </si>
-  <si>
-    <t>[{A, 442}]</t>
-  </si>
-  <si>
-    <t>{A, 442}</t>
-  </si>
-  <si>
-    <t>[{A, 564},{P,592}]</t>
-  </si>
-  <si>
-    <t>{A, 564}</t>
-  </si>
-  <si>
-    <t>[{P,592}, {P,681},{A, 686}]</t>
-  </si>
-  <si>
-    <t>{P,592}</t>
-  </si>
-  <si>
-    <t>[{P,681},{A, 686}]</t>
-  </si>
-  <si>
-    <t>{P,681}</t>
-  </si>
-  <si>
-    <t>[{A, 686}]</t>
-  </si>
-  <si>
-    <t>{A,686}</t>
-  </si>
-  <si>
-    <t>[{P,698},{A, 809}]</t>
+    <t>en marcha</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>lbda1</t>
+  </si>
+  <si>
+    <t>lbda2</t>
+  </si>
+  <si>
+    <t>tiempo  espera</t>
+  </si>
+  <si>
+    <t>atend</t>
+  </si>
+  <si>
+    <t>colasuben1</t>
+  </si>
+  <si>
+    <t>colasuben2</t>
+  </si>
+  <si>
+    <t>colabajan2</t>
+  </si>
+  <si>
+    <t>colasuben3</t>
+  </si>
+  <si>
+    <t>colabajan3</t>
+  </si>
+  <si>
+    <t>colabajan4</t>
+  </si>
+  <si>
+    <t>capAsc</t>
+  </si>
+  <si>
+    <t>pDestino</t>
+  </si>
+  <si>
+    <t>colaSalen1</t>
+  </si>
+  <si>
+    <t>colaSalen2</t>
+  </si>
+  <si>
+    <t>colaSalen3</t>
+  </si>
+  <si>
+    <t>colaSalen4</t>
+  </si>
+  <si>
+    <t>desppisos</t>
+  </si>
+  <si>
+    <t>ramdom lleg</t>
+  </si>
+  <si>
+    <t>ramdon dest</t>
+  </si>
+  <si>
+    <t>t en piso</t>
+  </si>
+  <si>
+    <t>[{P, 42}{A,121}]</t>
+  </si>
+  <si>
+    <t>{P,42}</t>
+  </si>
+  <si>
+    <t>[{A, 0}]</t>
   </si>
 </sst>
 </file>
@@ -404,7 +347,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -602,11 +545,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -620,13 +576,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,7 +613,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,117 +1308,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.85546875" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.140625" customWidth="1"/>
-    <col min="27" max="27" width="29.5703125" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2">
         <v>0.04</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2">
         <f ca="1">RAND()</f>
-        <v>0.50819805997890932</v>
+        <v>0.54715785535036043</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2">
         <f ca="1">ROUND(-(1/B1)*LOG($D$1, EXP(1)),0)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="I1" s="2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="L1" s="2">
         <v>4</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="N1" s="2">
         <v>20</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="P1" s="2">
         <v>100</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="2">
+        <v>1</v>
+      </c>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="R1" s="2">
-        <v>1</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="B2" s="2">
         <v>0.02</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2">
         <f ca="1">ROUND(-(1/B2)*LOG($D$1, EXP(1)),0)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
@@ -1464,19 +1420,19 @@
         <v>29</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F4" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>30</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>41</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -1484,13 +1440,13 @@
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
       <c r="M4" s="24" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="N4" s="25"/>
       <c r="O4" s="25"/>
       <c r="P4" s="26"/>
       <c r="Q4" s="24" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="R4" s="25"/>
       <c r="S4" s="25"/>
@@ -1498,16 +1454,17 @@
       <c r="U4" s="25"/>
       <c r="V4" s="26"/>
       <c r="W4" s="24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="X4" s="25"/>
       <c r="Y4" s="25"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="28"/>
       <c r="C5" s="23"/>
@@ -1515,52 +1472,52 @@
       <c r="E5" s="23"/>
       <c r="F5" s="27"/>
       <c r="G5" s="8" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="S5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="U5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="9" t="s">
+      <c r="V5" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="T5" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="U5" t="s">
-        <v>47</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="W5" s="12" t="s">
         <v>10</v>
@@ -1569,14 +1526,17 @@
         <v>12</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA5" s="21"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="Z5" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="21"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -1586,7 +1546,9 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
       <c r="G6" s="8">
         <v>0</v>
       </c>
@@ -1633,22 +1595,23 @@
         <v>4</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="W6" s="8"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1700,22 +1663,23 @@
         <v>1</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1767,22 +1731,23 @@
         <v>2</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="W8" s="8"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1834,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="W9" s="8">
         <v>1</v>
@@ -1843,24 +1808,27 @@
         <v>16</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>68</v>
+      <c r="B10" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1914,105 +1882,101 @@
       <c r="V10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="W10" s="8">
-        <v>1</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>0</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14">
-        <v>0</v>
-      </c>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
-      <c r="J11" s="14">
-        <v>0</v>
-      </c>
-      <c r="K11" s="14">
-        <v>1</v>
-      </c>
-      <c r="L11" s="17">
-        <v>1</v>
-      </c>
-      <c r="M11" s="16">
-        <v>0</v>
-      </c>
-      <c r="N11" s="14">
-        <v>0</v>
-      </c>
-      <c r="O11" s="14">
-        <v>0</v>
-      </c>
-      <c r="P11" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="16">
-        <v>9</v>
-      </c>
-      <c r="R11" s="14">
-        <v>9</v>
-      </c>
-      <c r="S11" s="14">
-        <v>1</v>
-      </c>
-      <c r="T11" s="14">
+      <c r="W10" s="8"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>0</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <v>1</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
+        <v>1</v>
+      </c>
+      <c r="L11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15">
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0</v>
+      </c>
+      <c r="O11" s="13">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>42</v>
+      </c>
+      <c r="R11" s="13">
+        <v>42</v>
+      </c>
+      <c r="S11" s="13">
+        <v>1</v>
+      </c>
+      <c r="T11" s="13">
         <v>2</v>
       </c>
-      <c r="U11" s="14">
+      <c r="U11" s="13">
         <v>2</v>
       </c>
-      <c r="V11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="W11" s="16">
-        <v>2</v>
-      </c>
-      <c r="X11" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y11" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z11" s="17">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="V11" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="W11" s="15">
+        <v>1</v>
+      </c>
+      <c r="X11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z11" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2070,802 +2034,354 @@
         <v>2</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>121</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>24</v>
-      </c>
-      <c r="R13" s="2">
-        <v>145</v>
-      </c>
-      <c r="S13" s="2">
-        <v>2</v>
-      </c>
-      <c r="T13" s="2">
-        <v>4</v>
-      </c>
-      <c r="U13" s="2">
-        <v>4</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="W13" s="2">
-        <v>3</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z13" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>145</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="W14" s="2">
-        <v>3</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>221</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>22</v>
-      </c>
-      <c r="R15" s="2">
-        <v>243</v>
-      </c>
-      <c r="S15" s="2">
-        <v>3</v>
-      </c>
-      <c r="T15" s="2">
-        <v>7</v>
-      </c>
-      <c r="U15" s="2">
-        <v>1</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W15" s="2">
-        <v>4</v>
-      </c>
-      <c r="X15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z15" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>243</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>2</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="W16" s="2">
-        <v>4</v>
-      </c>
-      <c r="X16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z16" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>321</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2">
-        <v>2</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>1</v>
-      </c>
-      <c r="N17" s="2">
-        <v>0</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>49</v>
-      </c>
-      <c r="R17" s="2">
-        <v>370</v>
-      </c>
-      <c r="S17" s="2">
-        <v>4</v>
-      </c>
-      <c r="T17" s="2">
-        <v>2</v>
-      </c>
-      <c r="U17" s="2">
-        <v>2</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W17" s="2">
-        <v>3</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>370</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>91</v>
-      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2">
-        <v>2</v>
-      </c>
-      <c r="L18" s="2">
-        <v>1</v>
-      </c>
-      <c r="M18" s="2">
-        <v>1</v>
-      </c>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2">
-        <v>0</v>
-      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="2">
-        <v>3</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>442</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>1</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2">
-        <v>1</v>
-      </c>
-      <c r="M19" s="2">
-        <v>2</v>
-      </c>
-      <c r="N19" s="2">
-        <v>1</v>
-      </c>
-      <c r="O19" s="2">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>150</v>
-      </c>
-      <c r="R19" s="2">
-        <v>592</v>
-      </c>
-      <c r="S19" s="2">
-        <v>3</v>
-      </c>
-      <c r="T19" s="2">
-        <v>5</v>
-      </c>
-      <c r="U19" s="2">
-        <v>1</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W19" s="2">
-        <v>2</v>
-      </c>
-      <c r="X19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z19" s="2">
-        <v>3</v>
-      </c>
-      <c r="AA19" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>564</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1</v>
-      </c>
-      <c r="M20" s="2">
-        <v>2</v>
-      </c>
-      <c r="N20" s="2">
-        <v>0</v>
-      </c>
-      <c r="O20" s="2">
-        <v>0</v>
-      </c>
-      <c r="P20" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>117</v>
-      </c>
-      <c r="R20" s="2">
-        <v>681</v>
-      </c>
-      <c r="S20" s="2">
-        <v>2</v>
-      </c>
-      <c r="T20" s="2">
-        <v>4</v>
-      </c>
-      <c r="U20" s="2">
-        <v>4</v>
-      </c>
-      <c r="V20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="W20" s="2">
-        <v>1</v>
-      </c>
-      <c r="X20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z20" s="2">
-        <v>2</v>
-      </c>
-      <c r="AA20" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>592</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
-      <c r="L21" s="2">
-        <v>1</v>
-      </c>
-      <c r="M21" s="2">
-        <v>2</v>
-      </c>
-      <c r="N21" s="2">
-        <v>0</v>
-      </c>
-      <c r="O21" s="2">
-        <v>0</v>
-      </c>
-      <c r="P21" s="2">
-        <v>0</v>
-      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2">
-        <v>1</v>
-      </c>
-      <c r="X21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z21" s="2">
-        <v>2</v>
-      </c>
-      <c r="AA21" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>681</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1</v>
-      </c>
-      <c r="M22" s="2">
-        <v>2</v>
-      </c>
-      <c r="N22" s="2">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2">
-        <v>0</v>
-      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="2">
-        <v>1</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z22" s="2">
-        <v>2</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>686</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2">
-        <v>1</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0</v>
-      </c>
-      <c r="N23" s="2">
-        <v>1</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>12</v>
-      </c>
-      <c r="R23" s="2">
-        <v>698</v>
-      </c>
-      <c r="S23" s="2">
-        <v>1</v>
-      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="2">
-        <v>2</v>
-      </c>
-      <c r="X23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2893,8 +2409,9 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB24" s="2"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2922,8 +2439,9 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB25" s="2"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2951,8 +2469,9 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB26" s="2"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2980,8 +2499,9 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB27" s="2"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3009,8 +2529,9 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB28" s="2"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3038,6 +2559,7 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3046,7 +2568,7 @@
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AB4:AB5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="G4:L4"/>

</xml_diff>

<commit_message>
Estructura general del LEF ok. LEF ordena los eventos conforme se insertan Falta: Programar evento persona Programar evento ascensor (puede presentar dificultad)
Despues:
Agregar las variables de desempeño y comenzar a mostrar resultados en GUI
</commit_message>
<xml_diff>
--- a/LEF Simulación.xlsx
+++ b/LEF Simulación.xlsx
@@ -705,36 +705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -747,6 +717,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,26 +1055,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="S3" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,21 +1479,21 @@
       </c>
       <c r="D1" s="2">
         <f ca="1">RAND()</f>
-        <v>0.35845478617861126</v>
+        <v>0.68288700774237776</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F1" s="2">
         <f ca="1">ROUND(-(1/B1)*LOG($D$1, EXP(1)),0)</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="I1" s="2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>70</v>
@@ -1534,68 +1534,68 @@
       </c>
       <c r="F2" s="2">
         <f ca="1">ROUND(-(1/B2)*LOG($D$1, EXP(1)),0)</f>
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="22" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="22" t="s">
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="22" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="27" t="s">
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="32" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="28"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="38"/>
       <c r="G5" s="7" t="s">
         <v>64</v>
       </c>
@@ -1623,7 +1623,7 @@
       <c r="O5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="26" t="s">
         <v>75</v>
       </c>
       <c r="Q5" s="9" t="s">
@@ -1638,7 +1638,7 @@
       <c r="T5" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="U5" s="31" t="s">
+      <c r="U5" s="21" t="s">
         <v>33</v>
       </c>
       <c r="V5" s="10" t="s">
@@ -1653,10 +1653,10 @@
       <c r="Y5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="29" t="s">
+      <c r="Z5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AA5" s="27"/>
+      <c r="AA5" s="32"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1701,22 +1701,22 @@
       <c r="P6" s="8">
         <v>0</v>
       </c>
-      <c r="Q6" s="37">
-        <v>0</v>
-      </c>
-      <c r="R6" s="38">
-        <v>0</v>
-      </c>
-      <c r="S6" s="38">
-        <v>1</v>
-      </c>
-      <c r="T6" s="38">
+      <c r="Q6" s="27">
+        <v>0</v>
+      </c>
+      <c r="R6" s="28">
+        <v>0</v>
+      </c>
+      <c r="S6" s="28">
+        <v>1</v>
+      </c>
+      <c r="T6" s="28">
         <v>4</v>
       </c>
-      <c r="U6" s="38">
+      <c r="U6" s="28">
         <v>4</v>
       </c>
-      <c r="V6" s="39" t="s">
+      <c r="V6" s="29" t="s">
         <v>44</v>
       </c>
       <c r="W6" s="7"/>
@@ -1768,22 +1768,22 @@
       <c r="P7" s="8">
         <v>0</v>
       </c>
-      <c r="Q7" s="37">
-        <v>0</v>
-      </c>
-      <c r="R7" s="38">
-        <v>0</v>
-      </c>
-      <c r="S7" s="38">
+      <c r="Q7" s="27">
+        <v>0</v>
+      </c>
+      <c r="R7" s="28">
+        <v>0</v>
+      </c>
+      <c r="S7" s="28">
         <v>2</v>
       </c>
-      <c r="T7" s="40">
+      <c r="T7" s="30">
         <v>7</v>
       </c>
-      <c r="U7" s="38">
-        <v>1</v>
-      </c>
-      <c r="V7" s="39" t="s">
+      <c r="U7" s="28">
+        <v>1</v>
+      </c>
+      <c r="V7" s="29" t="s">
         <v>51</v>
       </c>
       <c r="W7" s="7"/>
@@ -1835,22 +1835,22 @@
       <c r="P8" s="8">
         <v>0</v>
       </c>
-      <c r="Q8" s="37">
-        <v>0</v>
-      </c>
-      <c r="R8" s="38">
-        <v>0</v>
-      </c>
-      <c r="S8" s="38">
+      <c r="Q8" s="27">
+        <v>0</v>
+      </c>
+      <c r="R8" s="28">
+        <v>0</v>
+      </c>
+      <c r="S8" s="28">
         <v>3</v>
       </c>
-      <c r="T8" s="38">
+      <c r="T8" s="28">
         <v>2</v>
       </c>
-      <c r="U8" s="38">
+      <c r="U8" s="28">
         <v>2</v>
       </c>
-      <c r="V8" s="39" t="s">
+      <c r="V8" s="29" t="s">
         <v>51</v>
       </c>
       <c r="W8" s="7"/>
@@ -3076,172 +3076,172 @@
       <c r="AA29" s="6"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="G30" s="30"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="31"/>
-      <c r="U30" s="31"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="31"/>
-      <c r="Z30" s="32"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="22"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="21"/>
+      <c r="Z30" s="22"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="31"/>
-      <c r="S31" s="31"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="31"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="31"/>
-      <c r="Y31" s="31"/>
-      <c r="Z31" s="32"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="22"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="G32" s="30"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="31"/>
-      <c r="U32" s="31"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="31"/>
-      <c r="Z32" s="32"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="22"/>
     </row>
     <row r="33" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="31"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="31"/>
-      <c r="U33" s="31"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="31"/>
-      <c r="Z33" s="32"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="21"/>
+      <c r="Z33" s="22"/>
     </row>
     <row r="34" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G34" s="30"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="31"/>
-      <c r="U34" s="31"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="31"/>
-      <c r="Z34" s="32"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="21"/>
+      <c r="Z34" s="22"/>
     </row>
     <row r="35" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G35" s="30"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="31"/>
-      <c r="S35" s="31"/>
-      <c r="T35" s="31"/>
-      <c r="U35" s="31"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="31"/>
-      <c r="Y35" s="31"/>
-      <c r="Z35" s="32"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
+      <c r="Z35" s="22"/>
     </row>
     <row r="36" spans="7:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="35"/>
-      <c r="W36" s="33"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="35"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24"/>
+      <c r="Z36" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="W4:Z4"/>
     <mergeCell ref="AA4:AA5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="G4:L4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="W4:Z4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>